<commit_message>
output with updated ingredient/No more nonopioid
</commit_message>
<xml_diff>
--- a/RxNorm/Antidepressant/Active_Not_Found_Antidepressant.xlsx
+++ b/RxNorm/Antidepressant/Active_Not_Found_Antidepressant.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="32">
   <si>
     <t>rxcui</t>
   </si>
@@ -28,6 +28,27 @@
     <t>status</t>
   </si>
   <si>
+    <t>ingredients</t>
+  </si>
+  <si>
+    <t>selegiline hydrochloride 5 MG Oral Capsule</t>
+  </si>
+  <si>
+    <t>selegiline hydrochloride 1.25 MG Disintegrating Oral Tablet</t>
+  </si>
+  <si>
+    <t>selegiline hydrochloride 5 MG Oral Tablet</t>
+  </si>
+  <si>
+    <t>24 HR selegiline 0.25 MG/HR Transdermal System</t>
+  </si>
+  <si>
+    <t>24 HR selegiline 0.375 MG/HR Transdermal System</t>
+  </si>
+  <si>
+    <t>24 HR selegiline 0.5 MG/HR Transdermal System</t>
+  </si>
+  <si>
     <t>lithium carbonate 300 MG Oral Capsule</t>
   </si>
   <si>
@@ -71,6 +92,24 @@
   </si>
   <si>
     <t>Active</t>
+  </si>
+  <si>
+    <t>['selegiline']</t>
+  </si>
+  <si>
+    <t>['lithium carbonate']</t>
+  </si>
+  <si>
+    <t>['rasagiline']</t>
+  </si>
+  <si>
+    <t>['lithium aspartate']</t>
+  </si>
+  <si>
+    <t>['lithium citrate']</t>
+  </si>
+  <si>
+    <t>['lithium']</t>
   </si>
 </sst>
 </file>
@@ -428,13 +467,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -447,187 +486,331 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
+        <v>859186</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>859190</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>859193</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>865206</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>865210</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>865214</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
         <v>197889</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>197890</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>197891</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>197892</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>197893</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>199324</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>311355</v>
+      </c>
+      <c r="B14" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>608328</v>
+      </c>
+      <c r="B15" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
-        <v>197890</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
-        <v>197891</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
-        <v>197892</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>197893</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>199324</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
-        <v>311355</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <v>608328</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10">
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
         <v>636664</v>
       </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11">
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
         <v>746073</v>
       </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12">
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
         <v>749153</v>
       </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13">
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
         <v>756059</v>
       </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14">
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
         <v>846386</v>
       </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" t="s">
-        <v>18</v>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>